<commit_message>
Check values for date before cteating Calendar and Date instances in Application Startup Event Listener
</commit_message>
<xml_diff>
--- a/src/main/resources/data/globalterrorismdb_0919dist-mini2.xlsx
+++ b/src/main/resources/data/globalterrorismdb_0919dist-mini2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samsung\Spring\eclipse-workspace\Projects\GlobalTerrorismAPI\src\main\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samsung\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14C51761-632C-485B-96FF-745835FD4FAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4244FC-A33B-41A1-89D9-97C58A668D8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{8471290F-D369-4DC0-A1ED-126EB20088E5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="191">
   <si>
     <t>Unknown</t>
   </si>
@@ -601,6 +601,9 @@
   </si>
   <si>
     <t>The Wisconsin Cartographers' Guild, "Wisconsin's Past and Present: A Historical Atlas," The University of Wisconsin Press, 2002.</t>
+  </si>
+  <si>
+    <t>asd</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1009,7 @@
   <dimension ref="A1:EE200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2086,42 +2089,229 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:135" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="I5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AH5" s="13"/>
-      <c r="AJ5" s="13"/>
-      <c r="AL5" s="13"/>
-      <c r="AN5" s="13"/>
-      <c r="AP5" s="13"/>
-      <c r="AR5" s="13"/>
-      <c r="AT5" s="13"/>
-      <c r="AX5" s="13"/>
-      <c r="AZ5" s="13"/>
-      <c r="BB5" s="13"/>
-      <c r="BF5" s="13"/>
-      <c r="BG5" s="13"/>
-      <c r="BV5" s="13"/>
-      <c r="BY5" s="13"/>
-      <c r="CB5" s="13"/>
-      <c r="CE5" s="13"/>
-      <c r="CG5" s="13"/>
-      <c r="CI5" s="13"/>
-      <c r="CK5" s="13"/>
-      <c r="CM5" s="13"/>
-      <c r="CO5" s="13"/>
-      <c r="CQ5" s="13"/>
-      <c r="CS5" s="13"/>
-      <c r="CT5" s="13"/>
-      <c r="DC5" s="13"/>
-      <c r="DT5" s="13"/>
-      <c r="DZ5" s="13"/>
+    <row r="5" spans="1:135" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>197001020003</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5">
+        <v>-1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>217</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="N5">
+        <v>43.076591999999998</v>
+      </c>
+      <c r="O5">
+        <v>-89.412487999999996</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>175</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>7</v>
+      </c>
+      <c r="AD5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5">
+        <v>4</v>
+      </c>
+      <c r="AJ5" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="AK5">
+        <v>28</v>
+      </c>
+      <c r="AL5" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="AM5" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="AN5" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="AO5">
+        <v>217</v>
+      </c>
+      <c r="AP5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR5" s="2"/>
+      <c r="AT5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AZ5" s="2"/>
+      <c r="BB5" s="2"/>
+      <c r="BF5" s="2"/>
+      <c r="BG5" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="BM5" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="BN5">
+        <v>0</v>
+      </c>
+      <c r="BQ5">
+        <v>0</v>
+      </c>
+      <c r="BR5">
+        <v>1</v>
+      </c>
+      <c r="BS5">
+        <v>1</v>
+      </c>
+      <c r="BT5">
+        <v>1</v>
+      </c>
+      <c r="BU5">
+        <v>1</v>
+      </c>
+      <c r="BV5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="BY5" s="2"/>
+      <c r="CB5" s="2"/>
+      <c r="CD5">
+        <v>8</v>
+      </c>
+      <c r="CE5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="CF5">
+        <v>19</v>
+      </c>
+      <c r="CG5" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="CI5" s="2"/>
+      <c r="CK5" s="2"/>
+      <c r="CM5" s="2"/>
+      <c r="CO5" s="2"/>
+      <c r="CQ5" s="2"/>
+      <c r="CS5" s="2"/>
+      <c r="CT5" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="CU5">
+        <v>0</v>
+      </c>
+      <c r="CV5">
+        <v>0</v>
+      </c>
+      <c r="CW5">
+        <v>0</v>
+      </c>
+      <c r="CX5">
+        <v>0</v>
+      </c>
+      <c r="CY5">
+        <v>0</v>
+      </c>
+      <c r="CZ5">
+        <v>0</v>
+      </c>
+      <c r="DA5">
+        <v>1</v>
+      </c>
+      <c r="DB5">
+        <v>3</v>
+      </c>
+      <c r="DC5" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="DD5">
+        <v>60000</v>
+      </c>
+      <c r="DE5" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="DF5">
+        <v>0</v>
+      </c>
+      <c r="DM5">
+        <v>0</v>
+      </c>
+      <c r="DT5" s="2"/>
+      <c r="DV5" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="DW5" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="DX5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="DY5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="DZ5" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="EA5">
+        <v>0</v>
+      </c>
+      <c r="EB5">
+        <v>0</v>
+      </c>
+      <c r="EC5">
+        <v>0</v>
+      </c>
+      <c r="ED5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:135" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>

</xml_diff>

<commit_message>
Convert numeric values to boolean in Application Startup Event Listener
</commit_message>
<xml_diff>
--- a/src/main/resources/data/globalterrorismdb_0919dist-mini2.xlsx
+++ b/src/main/resources/data/globalterrorismdb_0919dist-mini2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samsung\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4244FC-A33B-41A1-89D9-97C58A668D8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5031639B-5686-4757-9C3B-3FA5D57CB77E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{8471290F-D369-4DC0-A1ED-126EB20088E5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="190">
   <si>
     <t>Unknown</t>
   </si>
@@ -601,9 +601,6 @@
   </si>
   <si>
     <t>The Wisconsin Cartographers' Guild, "Wisconsin's Past and Present: A Historical Atlas," The University of Wisconsin Press, 2002.</t>
-  </si>
-  <si>
-    <t>asd</t>
   </si>
 </sst>
 </file>
@@ -1008,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3F4CFC-A9DF-4A58-AE25-FA62AD0E6FFF}">
   <dimension ref="A1:EE200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1487,13 +1484,13 @@
       </c>
       <c r="Y2" s="2"/>
       <c r="Z2" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="8">
         <v>1</v>
       </c>
       <c r="AB2" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC2">
         <v>2</v>
@@ -1711,7 +1708,7 @@
         <v>166</v>
       </c>
       <c r="Z3" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA3" s="8">
         <v>1</v>
@@ -1931,7 +1928,7 @@
         <v>1</v>
       </c>
       <c r="AB4" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC4">
         <v>7</v>
@@ -2090,228 +2087,53 @@
       </c>
     </row>
     <row r="5" spans="1:135" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>197001020003</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="D5">
-        <v>-1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>217</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="N5">
-        <v>43.076591999999998</v>
-      </c>
-      <c r="O5">
-        <v>-89.412487999999996</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="S5" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5">
-        <v>1</v>
-      </c>
-      <c r="V5">
-        <v>1</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="12"/>
+      <c r="I5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="S5" s="10"/>
       <c r="Y5" s="2"/>
-      <c r="Z5" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="8">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <v>7</v>
-      </c>
-      <c r="AD5" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AD5" s="2"/>
       <c r="AF5" s="2"/>
       <c r="AH5" s="2"/>
-      <c r="AI5">
-        <v>4</v>
-      </c>
-      <c r="AJ5" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="AK5">
-        <v>28</v>
-      </c>
-      <c r="AL5" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="AM5" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="AN5" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="AO5">
-        <v>217</v>
-      </c>
-      <c r="AP5" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="AJ5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="10"/>
+      <c r="AP5" s="2"/>
       <c r="AR5" s="2"/>
       <c r="AT5" s="2"/>
       <c r="AX5" s="2"/>
       <c r="AZ5" s="2"/>
       <c r="BB5" s="2"/>
       <c r="BF5" s="2"/>
-      <c r="BG5" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="BM5" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="BN5">
-        <v>0</v>
-      </c>
-      <c r="BQ5">
-        <v>0</v>
-      </c>
-      <c r="BR5">
-        <v>1</v>
-      </c>
-      <c r="BS5">
-        <v>1</v>
-      </c>
-      <c r="BT5">
-        <v>1</v>
-      </c>
-      <c r="BU5">
-        <v>1</v>
-      </c>
-      <c r="BV5" s="2" t="s">
-        <v>182</v>
-      </c>
+      <c r="BG5" s="2"/>
+      <c r="BM5" s="10"/>
+      <c r="BV5" s="2"/>
       <c r="BY5" s="2"/>
       <c r="CB5" s="2"/>
-      <c r="CD5">
-        <v>8</v>
-      </c>
-      <c r="CE5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="CF5">
-        <v>19</v>
-      </c>
-      <c r="CG5" s="2" t="s">
-        <v>183</v>
-      </c>
+      <c r="CE5" s="2"/>
+      <c r="CG5" s="2"/>
       <c r="CI5" s="2"/>
       <c r="CK5" s="2"/>
       <c r="CM5" s="2"/>
       <c r="CO5" s="2"/>
       <c r="CQ5" s="2"/>
       <c r="CS5" s="2"/>
-      <c r="CT5" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="CU5">
-        <v>0</v>
-      </c>
-      <c r="CV5">
-        <v>0</v>
-      </c>
-      <c r="CW5">
-        <v>0</v>
-      </c>
-      <c r="CX5">
-        <v>0</v>
-      </c>
-      <c r="CY5">
-        <v>0</v>
-      </c>
-      <c r="CZ5">
-        <v>0</v>
-      </c>
-      <c r="DA5">
-        <v>1</v>
-      </c>
-      <c r="DB5">
-        <v>3</v>
-      </c>
-      <c r="DC5" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="DD5">
-        <v>60000</v>
-      </c>
-      <c r="DE5" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="DF5">
-        <v>0</v>
-      </c>
-      <c r="DM5">
-        <v>0</v>
-      </c>
+      <c r="CT5" s="2"/>
+      <c r="DC5" s="2"/>
+      <c r="DE5" s="2"/>
       <c r="DT5" s="2"/>
-      <c r="DV5" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="DW5" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="DX5" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="DY5" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="DZ5" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="EA5">
-        <v>0</v>
-      </c>
-      <c r="EB5">
-        <v>0</v>
-      </c>
-      <c r="EC5">
-        <v>0</v>
-      </c>
-      <c r="ED5">
-        <v>0</v>
-      </c>
+      <c r="DV5" s="2"/>
+      <c r="DW5" s="2"/>
+      <c r="DX5" s="2"/>
+      <c r="DY5" s="2"/>
+      <c r="DZ5" s="2"/>
     </row>
     <row r="6" spans="1:135" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11"/>

</xml_diff>

<commit_message>
Create Event from data loaded from file in Application Startup Event Listener
</commit_message>
<xml_diff>
--- a/src/main/resources/data/globalterrorismdb_0919dist-mini2.xlsx
+++ b/src/main/resources/data/globalterrorismdb_0919dist-mini2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samsung\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5031639B-5686-4757-9C3B-3FA5D57CB77E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F25169-E87D-454A-8CD7-DD882F5275F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15600" xr2:uid="{8471290F-D369-4DC0-A1ED-126EB20088E5}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="196">
   <si>
     <t>Unknown</t>
   </si>
@@ -601,6 +601,24 @@
   </si>
   <si>
     <t>The Wisconsin Cartographers' Guild, "Wisconsin's Past and Present: A Historical Atlas," The University of Wisconsin Press, 2002.</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -1005,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F3F4CFC-A9DF-4A58-AE25-FA62AD0E6FFF}">
   <dimension ref="A1:EE200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
+      <selection activeCell="BP2" sqref="BP2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1533,11 +1551,29 @@
       <c r="BG2" s="2" t="s">
         <v>151</v>
       </c>
+      <c r="BI2" t="s">
+        <v>190</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>191</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>192</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>193</v>
+      </c>
       <c r="BM2" s="10" t="s">
         <v>152</v>
       </c>
       <c r="BN2">
         <v>0</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>195</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>194</v>
       </c>
       <c r="BQ2">
         <v>0</v>
@@ -1757,9 +1793,27 @@
       <c r="BG3" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="BI3" t="s">
+        <v>190</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>191</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>192</v>
+      </c>
+      <c r="BL3" t="s">
+        <v>193</v>
+      </c>
       <c r="BM3" s="8"/>
       <c r="BN3">
         <v>0</v>
+      </c>
+      <c r="BO3" t="s">
+        <v>195</v>
+      </c>
+      <c r="BP3" t="s">
+        <v>194</v>
       </c>
       <c r="BQ3">
         <v>0</v>
@@ -1971,11 +2025,29 @@
       <c r="BG4" s="2" t="s">
         <v>180</v>
       </c>
+      <c r="BI4" t="s">
+        <v>190</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>191</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>192</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>193</v>
+      </c>
       <c r="BM4" s="10" t="s">
         <v>181</v>
       </c>
       <c r="BN4">
         <v>0</v>
+      </c>
+      <c r="BO4" t="s">
+        <v>195</v>
+      </c>
+      <c r="BP4" t="s">
+        <v>194</v>
       </c>
       <c r="BQ4">
         <v>0</v>

</xml_diff>